<commit_message>
Correct tab 3 results in flatten ex xls
</commit_message>
<xml_diff>
--- a/misc/Lateral Flatten Example.xlsx
+++ b/misc/Lateral Flatten Example.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="75">
   <si>
     <t>select $1</t>
   </si>
@@ -120,13 +120,13 @@
     <t>Account Number</t>
   </si>
   <si>
-    <t>['Account Number']</t>
+    <t>['Event Details']['Account Number']</t>
   </si>
   <si>
     <t>Account Type</t>
   </si>
   <si>
-    <t>['Account Type']</t>
+    <t>['Event Details']['Account Type']</t>
   </si>
   <si>
     <t>Premier Savings</t>
@@ -135,19 +135,19 @@
     <t>Current Balance</t>
   </si>
   <si>
-    <t>['Current Balance']</t>
+    <t>['Event Details']['Current Balance']</t>
   </si>
   <si>
     <t>Recent Txns</t>
   </si>
   <si>
-    <t>['Recent Txns']</t>
+    <t>['Event Details']['Recent Txns']</t>
   </si>
   <si>
     <t>[   {     "Amount": 897.08,     "Date": "2023-05-29",     "Type": "POS Debit"   },   {     "Amount": 970.02,     "Date": "2023-04-22",     "Type": "ACH Debit"   },   {     "Amount": 1736.41,     "Date": "2023-05-10",     "Type": "Check Deposit"   },   {     "Amount": 769.25,     "Date": "2023-04-25",     "Type": "Check Credit"   },   {     "Amount": 1065.84,     "Date": "2023-04-20",     "Type": "POS Debit"   } ]</t>
   </si>
   <si>
-    <t>['Recent Txns'][0]</t>
+    <t>['Event Details']['Recent Txns'][0]</t>
   </si>
   <si>
     <t>{   "Amount": 897.08,   "Date": "2023-05-29",   "Type": "POS Debit" }</t>
@@ -156,88 +156,88 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>['Recent Txns'][0].Amount</t>
+    <t>['Event Details']['Recent Txns'][0].Amount</t>
   </si>
   <si>
-    <t>['Recent Txns'][0].Date</t>
+    <t>['Event Details']['Recent Txns'][0].Date</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>['Recent Txns'][0].Type</t>
+    <t>['Event Details']['Recent Txns'][0].Type</t>
   </si>
   <si>
     <t>POS Debit</t>
   </si>
   <si>
-    <t>['Recent Txns'][1]</t>
+    <t>['Event Details']['Recent Txns'][1]</t>
   </si>
   <si>
     <t>{   "Amount": 970.02,   "Date": "2023-04-22",   "Type": "ACH Debit" }</t>
   </si>
   <si>
-    <t>['Recent Txns'][1].Amount</t>
+    <t>['Event Details']['Recent Txns'][1].Amount</t>
   </si>
   <si>
-    <t>['Recent Txns'][1].Date</t>
+    <t>['Event Details']['Recent Txns'][1].Date</t>
   </si>
   <si>
-    <t>['Recent Txns'][1].Type</t>
+    <t>['Event Details']['Recent Txns'][1].Type</t>
   </si>
   <si>
     <t>ACH Debit</t>
   </si>
   <si>
-    <t>['Recent Txns'][2]</t>
+    <t>['Event Details']['Recent Txns'][2]</t>
   </si>
   <si>
     <t>{   "Amount": 1736.41,   "Date": "2023-05-10",   "Type": "Check Deposit" }</t>
   </si>
   <si>
-    <t>['Recent Txns'][2].Amount</t>
+    <t>['Event Details']['Recent Txns'][2].Amount</t>
   </si>
   <si>
-    <t>['Recent Txns'][2].Date</t>
+    <t>['Event Details']['Recent Txns'][2].Date</t>
   </si>
   <si>
-    <t>['Recent Txns'][2].Type</t>
+    <t>['Event Details']['Recent Txns'][2].Type</t>
   </si>
   <si>
     <t>Check Deposit</t>
   </si>
   <si>
-    <t>['Recent Txns'][3]</t>
+    <t>['Event Details']['Recent Txns'][3]</t>
   </si>
   <si>
     <t>{   "Amount": 769.25,   "Date": "2023-04-25",   "Type": "Check Credit" }</t>
   </si>
   <si>
-    <t>['Recent Txns'][3].Amount</t>
+    <t>['Event Details']['Recent Txns'][3].Amount</t>
   </si>
   <si>
-    <t>['Recent Txns'][3].Date</t>
+    <t>['Event Details']['Recent Txns'][3].Date</t>
   </si>
   <si>
-    <t>['Recent Txns'][3].Type</t>
+    <t>['Event Details']['Recent Txns'][3].Type</t>
   </si>
   <si>
     <t>Check Credit</t>
   </si>
   <si>
-    <t>['Recent Txns'][4]</t>
+    <t>['Event Details']['Recent Txns'][4]</t>
   </si>
   <si>
     <t>{   "Amount": 1065.84,   "Date": "2023-04-20",   "Type": "POS Debit" }</t>
   </si>
   <si>
-    <t>['Recent Txns'][4].Amount</t>
+    <t>['Event Details']['Recent Txns'][4].Amount</t>
   </si>
   <si>
-    <t>['Recent Txns'][4].Date</t>
+    <t>['Event Details']['Recent Txns'][4].Date</t>
   </si>
   <si>
-    <t>['Recent Txns'][4].Type</t>
+    <t>['Event Details']['Recent Txns'][4].Type</t>
   </si>
 </sst>
 </file>
@@ -4034,16 +4034,16 @@
         <v>1.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4">
-        <v>4.430596594E9</v>
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G11" s="3" t="b">
         <v>0</v>
@@ -4057,16 +4057,16 @@
         <v>1.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>38</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="6">
+        <v>45053.0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G12" s="3" t="b">
         <v>0</v>
@@ -4080,19 +4080,19 @@
         <v>1.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="4">
-        <v>976879.58</v>
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G13" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="3" t="b">
         <v>0</v>
@@ -4103,13 +4103,13 @@
         <v>1.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4.430596594E9</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>26</v>
@@ -4118,27 +4118,28 @@
         <v>0</v>
       </c>
       <c r="H14" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3">
         <v>1.0</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.0</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="G15" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="3" t="b">
         <v>0</v>
@@ -4149,16 +4150,16 @@
         <v>1.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E16" s="4">
-        <v>897.08</v>
+        <v>976879.58</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="G16" s="3" t="b">
         <v>0</v>
@@ -4172,42 +4173,43 @@
         <v>1.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="6">
-        <v>45075.0</v>
+        <v>42</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="G17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="H17" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3">
         <v>1.0</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.0</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G18" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="3" t="b">
         <v>0</v>
@@ -4217,20 +4219,21 @@
       <c r="A19" s="3">
         <v>1.0</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4">
+        <v>897.08</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G19" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="3" t="b">
         <v>0</v>
@@ -4241,16 +4244,16 @@
         <v>1.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="4">
-        <v>970.02</v>
+        <v>48</v>
+      </c>
+      <c r="E20" s="6">
+        <v>45075.0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G20" s="3" t="b">
         <v>0</v>
@@ -4264,16 +4267,16 @@
         <v>1.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="6">
-        <v>45038.0</v>
+        <v>50</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G21" s="3" t="b">
         <v>0</v>
@@ -4286,20 +4289,21 @@
       <c r="A22" s="3">
         <v>1.0</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1.0</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G22" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="3" t="b">
         <v>0</v>
@@ -4309,20 +4313,21 @@
       <c r="A23" s="3">
         <v>1.0</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4">
+        <v>970.02</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G23" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="3" t="b">
         <v>0</v>
@@ -4333,16 +4338,16 @@
         <v>1.0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="4">
-        <v>1736.41</v>
+        <v>55</v>
+      </c>
+      <c r="E24" s="6">
+        <v>45038.0</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G24" s="3" t="b">
         <v>0</v>
@@ -4356,16 +4361,16 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="6">
-        <v>45056.0</v>
+        <v>56</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G25" s="3" t="b">
         <v>0</v>
@@ -4378,20 +4383,21 @@
       <c r="A26" s="3">
         <v>1.0</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2.0</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G26" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="3" t="b">
         <v>0</v>
@@ -4401,20 +4407,21 @@
       <c r="A27" s="3">
         <v>1.0</v>
       </c>
+      <c r="B27" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4">
+        <v>1736.41</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="G27" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="3" t="b">
         <v>0</v>
@@ -4425,16 +4432,16 @@
         <v>1.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="4">
-        <v>769.25</v>
+        <v>61</v>
+      </c>
+      <c r="E28" s="6">
+        <v>45056.0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G28" s="3" t="b">
         <v>0</v>
@@ -4448,16 +4455,16 @@
         <v>1.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="6">
-        <v>45041.0</v>
+        <v>62</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G29" s="3" t="b">
         <v>0</v>
@@ -4470,20 +4477,21 @@
       <c r="A30" s="3">
         <v>1.0</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3.0</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="G30" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="3" t="b">
         <v>0</v>
@@ -4493,20 +4501,21 @@
       <c r="A31" s="3">
         <v>1.0</v>
       </c>
+      <c r="B31" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C31" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
+        <v>769.25</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="G31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="3" t="b">
         <v>0</v>
@@ -4517,16 +4526,16 @@
         <v>1.0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="4">
-        <v>1065.84</v>
+        <v>67</v>
+      </c>
+      <c r="E32" s="6">
+        <v>45041.0</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G32" s="3" t="b">
         <v>0</v>
@@ -4540,16 +4549,16 @@
         <v>1.0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="6">
-        <v>45036.0</v>
+        <v>68</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G33" s="3" t="b">
         <v>0</v>
@@ -4562,42 +4571,163 @@
       <c r="A34" s="3">
         <v>1.0</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D34" s="3">
+        <v>4.0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="G34" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="E35" s="8"/>
+      <c r="A35" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1065.84</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
-      <c r="E36" s="8"/>
+      <c r="A36" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="6">
+        <v>45036.0</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
-      <c r="E37" s="8"/>
+      <c r="A37" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
-      <c r="E38" s="8"/>
+      <c r="A38" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
-      <c r="E39" s="8"/>
+      <c r="A39" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.308912037037037</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="E40" s="8"/>
+      <c r="A40" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="E41" s="8"/>

</xml_diff>